<commit_message>
Atualização dados financeiros - Outubro 2025
- Atualizado modulo_fechamento_mes.py com dados de outubro:
  * Faturamento: R$ 159.565,41 (104 transações)
  * Caixa recebido: R$ 122.540,21 (Pagar.me)
  * Taxas pagas: R$ 13.299,11
  * Chargebacks: R$ 2.157,84

- Atualizado modulo_fluxo_caixa.py com saldos de 05/11/2025:
  * Total em conta: R$ 495.330,60
  * Total a receber: R$ 231.736,87

- Ajustado Matriz financeira.xlsx:
  * Removido Prolabore (R$ 30k) das despesas
  * Adicionado Antecipação de Dividendos pós-resultado
  * Resultado Líquido Outubro: R$ 64.198,70

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Matriz financeira.xlsx
+++ b/Matriz financeira.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BQ56"/>
+  <dimension ref="A1:BQ58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -746,7 +746,9 @@
       <c r="F3" t="n">
         <v>257074.18</v>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="n">
+        <v>159565.41</v>
+      </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -827,9 +829,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
-        <v>198000</v>
-      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
         <v>217800.0000000001</v>
       </c>
@@ -1028,9 +1028,7 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="n">
-        <v>50000</v>
-      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
         <v>50000</v>
       </c>
@@ -1238,7 +1236,7 @@
         <v>257074.18</v>
       </c>
       <c r="G6" t="n">
-        <v>248000</v>
+        <v>159565.41</v>
       </c>
       <c r="H6" t="n">
         <v>267800.0000000001</v>
@@ -1593,7 +1591,7 @@
         <v>8354.91085</v>
       </c>
       <c r="G9" t="n">
-        <v>8060.000000000001</v>
+        <v>5185.875825</v>
       </c>
       <c r="H9" t="n">
         <v>8703.500000000002</v>
@@ -1796,7 +1794,7 @@
         <v>40815.23</v>
       </c>
       <c r="G10" t="n">
-        <v>20608.8</v>
+        <v>13259.885571</v>
       </c>
       <c r="H10" t="n">
         <v>22254.18000000001</v>
@@ -2005,7 +2003,7 @@
         <v>49170.14085</v>
       </c>
       <c r="G11" t="n">
-        <v>28668.8</v>
+        <v>18445.761396</v>
       </c>
       <c r="H11" t="n">
         <v>30957.68000000001</v>
@@ -2360,7 +2358,7 @@
         <v>2604</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>206.11</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -2723,7 +2721,7 @@
         <v>6576.24</v>
       </c>
       <c r="G17" t="n">
-        <v>67360</v>
+        <v>21606.51</v>
       </c>
       <c r="H17" t="n">
         <v>18746.00000000001</v>
@@ -2932,7 +2930,7 @@
         <v>6576.24</v>
       </c>
       <c r="G18" t="n">
-        <v>17360</v>
+        <v>5283.659999999999</v>
       </c>
       <c r="H18" t="n">
         <v>18746.00000000001</v>
@@ -3133,7 +3131,7 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="n">
-        <v>30000</v>
+        <v>16322.85</v>
       </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
@@ -3237,9 +3235,7 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
-      <c r="G20" t="n">
-        <v>20000</v>
-      </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
@@ -3339,7 +3335,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>24800</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
         <v>26780.00000000001</v>
@@ -3539,9 +3535,7 @@
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
-      <c r="G22" t="n">
-        <v>24800</v>
-      </c>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="n">
         <v>26780.00000000001</v>
       </c>
@@ -3749,7 +3743,7 @@
         <v>33419.6434</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>20743.5033</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -3957,7 +3951,9 @@
       <c r="F24" t="n">
         <v>33419.6434</v>
       </c>
-      <c r="G24" t="inlineStr"/>
+      <c r="G24" t="n">
+        <v>20743.5033</v>
+      </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
@@ -4041,7 +4037,7 @@
         <v>2289.01</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -4841,12 +4837,8 @@
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
-      <c r="G32" t="n">
-        <v>60000</v>
-      </c>
-      <c r="H32" t="n">
-        <v>60000</v>
-      </c>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
       <c r="I32" t="n">
         <v>120000</v>
       </c>
@@ -5051,7 +5043,7 @@
         <v>4000</v>
       </c>
       <c r="G33" t="n">
-        <v>6500</v>
+        <v>4000</v>
       </c>
       <c r="H33" t="n">
         <v>6500</v>
@@ -5466,9 +5458,7 @@
         <v>0</v>
       </c>
       <c r="F35" t="inlineStr"/>
-      <c r="G35" t="n">
-        <v>2500</v>
-      </c>
+      <c r="G35" t="inlineStr"/>
       <c r="H35" t="n">
         <v>2500</v>
       </c>
@@ -5676,7 +5666,7 @@
         <v>37557.41800000001</v>
       </c>
       <c r="G36" t="n">
-        <v>51650</v>
+        <v>27674.84</v>
       </c>
       <c r="H36" t="n">
         <v>60630.00000000001</v>
@@ -5885,7 +5875,7 @@
         <v>25707.418</v>
       </c>
       <c r="G37" t="n">
-        <v>24800</v>
+        <v>10824.84</v>
       </c>
       <c r="H37" t="n">
         <v>26780.00000000001</v>
@@ -6512,7 +6502,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="H40" t="n">
         <v>5000</v>
@@ -6717,7 +6707,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="H41" t="n">
         <v>5000</v>
@@ -6926,7 +6916,7 @@
         <v>4365.820000000001</v>
       </c>
       <c r="G42" t="n">
-        <v>4365.820000000001</v>
+        <v>2609.990000000001</v>
       </c>
       <c r="H42" t="n">
         <v>4365.820000000001</v>
@@ -7343,9 +7333,7 @@
       <c r="F44" t="n">
         <v>60.3</v>
       </c>
-      <c r="G44" t="n">
-        <v>60.3</v>
-      </c>
+      <c r="G44" t="inlineStr"/>
       <c r="H44" t="n">
         <v>60.3</v>
       </c>
@@ -7552,9 +7540,7 @@
       <c r="F45" t="n">
         <v>146.68</v>
       </c>
-      <c r="G45" t="n">
-        <v>146.68</v>
-      </c>
+      <c r="G45" t="inlineStr"/>
       <c r="H45" t="n">
         <v>146.68</v>
       </c>
@@ -8180,7 +8166,7 @@
         <v>2250.25</v>
       </c>
       <c r="G48" t="n">
-        <v>2250.25</v>
+        <v>1214.65</v>
       </c>
       <c r="H48" t="n">
         <v>2250.25</v>
@@ -8388,9 +8374,7 @@
       <c r="F49" t="n">
         <v>269.54</v>
       </c>
-      <c r="G49" t="n">
-        <v>269.54</v>
-      </c>
+      <c r="G49" t="inlineStr"/>
       <c r="H49" t="n">
         <v>269.54</v>
       </c>
@@ -8806,9 +8790,7 @@
       <c r="F51" t="n">
         <v>241.7</v>
       </c>
-      <c r="G51" t="n">
-        <v>241.7</v>
-      </c>
+      <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
         <v>241.7</v>
       </c>
@@ -9016,7 +8998,7 @@
         <v>111.31</v>
       </c>
       <c r="G52" t="n">
-        <v>111.31</v>
+        <v>109.3</v>
       </c>
       <c r="H52" t="n">
         <v>111.31</v>
@@ -9219,13 +9201,13 @@
         <v>30049.88</v>
       </c>
       <c r="E53" t="n">
-        <v>41557.21</v>
+        <v>59990.91503975</v>
       </c>
       <c r="F53" t="n">
-        <v>57392.488</v>
+        <v>90812.13140000001</v>
       </c>
       <c r="G53" t="n">
-        <v>214675.82</v>
+        <v>76920.95329999999</v>
       </c>
       <c r="H53" t="n">
         <v>177021.82</v>
@@ -9499,25 +9481,25 @@
         <v>388701.977888</v>
       </c>
       <c r="E55" t="n">
-        <v>100240.521075</v>
+        <v>81806.81603525</v>
       </c>
       <c r="F55" t="n">
-        <v>150511.55115</v>
+        <v>117091.90775</v>
       </c>
       <c r="G55" t="n">
-        <v>4655.380000000005</v>
+        <v>64198.69530399999</v>
       </c>
       <c r="H55" t="n">
-        <v>59820.50000000006</v>
+        <v>59820.50000000009</v>
       </c>
       <c r="I55" t="n">
-        <v>13202.13200000004</v>
+        <v>13202.13200000007</v>
       </c>
       <c r="J55" t="n">
         <v>12921.92720000003</v>
       </c>
       <c r="K55" t="n">
-        <v>33305.81456000009</v>
+        <v>33305.81455999997</v>
       </c>
       <c r="L55" t="n">
         <v>41806.49628800008</v>
@@ -9535,10 +9517,10 @@
         <v>41277.44716254098</v>
       </c>
       <c r="Q55" t="n">
-        <v>48126.71052066801</v>
+        <v>48126.71052066807</v>
       </c>
       <c r="R55" t="n">
-        <v>64806.43704670138</v>
+        <v>64806.43704670132</v>
       </c>
       <c r="S55" t="n">
         <v>76767.74989903648</v>
@@ -9553,7 +9535,7 @@
         <v>39505.19060437207</v>
       </c>
       <c r="W55" t="n">
-        <v>54044.24113459082</v>
+        <v>54044.24113459088</v>
       </c>
       <c r="X55" t="n">
         <v>95030.24419132038</v>
@@ -9565,7 +9547,7 @@
         <v>125890.3157709307</v>
       </c>
       <c r="AA55" t="n">
-        <v>143562.6225594772</v>
+        <v>143562.6225594773</v>
       </c>
       <c r="AB55" t="n">
         <v>112118.5446874512</v>
@@ -9583,7 +9565,7 @@
         <v>196095.8057423763</v>
       </c>
       <c r="AG55" t="n">
-        <v>269778.3870294951</v>
+        <v>269778.387029495</v>
       </c>
       <c r="AH55" t="n">
         <v>277238.4001349375</v>
@@ -9595,25 +9577,25 @@
         <v>292495.8054385158</v>
       </c>
       <c r="AK55" t="n">
-        <v>115296.5798200937</v>
+        <v>115296.5798200932</v>
       </c>
       <c r="AL55" t="n">
-        <v>293214.3658173948</v>
+        <v>293214.3658173947</v>
       </c>
       <c r="AM55" t="n">
-        <v>301250.9186046557</v>
+        <v>301250.9186046552</v>
       </c>
       <c r="AN55" t="n">
-        <v>279408.0196837253</v>
+        <v>279408.0196837258</v>
       </c>
       <c r="AO55" t="n">
-        <v>317687.4772789812</v>
+        <v>317687.4772789814</v>
       </c>
       <c r="AP55" t="n">
-        <v>323289.910251771</v>
+        <v>323289.9102517708</v>
       </c>
       <c r="AQ55" t="n">
-        <v>328948.3675542888</v>
+        <v>328948.3675542892</v>
       </c>
       <c r="AR55" t="n">
         <v>304663.4094298319</v>
@@ -9622,37 +9604,37 @@
         <v>340435.6017241301</v>
       </c>
       <c r="AT55" t="n">
-        <v>346265.5159413714</v>
+        <v>346265.5159413712</v>
       </c>
       <c r="AU55" t="n">
-        <v>352153.7293007852</v>
+        <v>352153.7293007857</v>
       </c>
       <c r="AV55" t="n">
-        <v>358100.824793793</v>
+        <v>358100.8247937926</v>
       </c>
       <c r="AW55" t="n">
-        <v>194107.3912417309</v>
+        <v>194107.3912417304</v>
       </c>
       <c r="AX55" t="n">
-        <v>370174.0233541484</v>
+        <v>370174.0233541486</v>
       </c>
       <c r="AY55" t="n">
         <v>376301.3217876897</v>
       </c>
       <c r="AZ55" t="n">
-        <v>352489.8932055668</v>
+        <v>352489.893205567</v>
       </c>
       <c r="BA55" t="n">
         <v>388740.3503376223</v>
       </c>
       <c r="BB55" t="n">
-        <v>395053.3120409987</v>
+        <v>395053.3120409985</v>
       </c>
       <c r="BC55" t="n">
-        <v>401429.4033614087</v>
+        <v>401429.403361409</v>
       </c>
       <c r="BD55" t="n">
-        <v>377869.2555950226</v>
+        <v>377869.255595023</v>
       </c>
       <c r="BE55" t="n">
         <v>414373.5063509729</v>
@@ -9903,6 +9885,158 @@
         <v>33.99</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
+      <c r="R57" t="inlineStr"/>
+      <c r="S57" t="inlineStr"/>
+      <c r="T57" t="inlineStr"/>
+      <c r="U57" t="inlineStr"/>
+      <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr"/>
+      <c r="Y57" t="inlineStr"/>
+      <c r="Z57" t="inlineStr"/>
+      <c r="AA57" t="inlineStr"/>
+      <c r="AB57" t="inlineStr"/>
+      <c r="AC57" t="inlineStr"/>
+      <c r="AD57" t="inlineStr"/>
+      <c r="AE57" t="inlineStr"/>
+      <c r="AF57" t="inlineStr"/>
+      <c r="AG57" t="inlineStr"/>
+      <c r="AH57" t="inlineStr"/>
+      <c r="AI57" t="inlineStr"/>
+      <c r="AJ57" t="inlineStr"/>
+      <c r="AK57" t="inlineStr"/>
+      <c r="AL57" t="inlineStr"/>
+      <c r="AM57" t="inlineStr"/>
+      <c r="AN57" t="inlineStr"/>
+      <c r="AO57" t="inlineStr"/>
+      <c r="AP57" t="inlineStr"/>
+      <c r="AQ57" t="inlineStr"/>
+      <c r="AR57" t="inlineStr"/>
+      <c r="AS57" t="inlineStr"/>
+      <c r="AT57" t="inlineStr"/>
+      <c r="AU57" t="inlineStr"/>
+      <c r="AV57" t="inlineStr"/>
+      <c r="AW57" t="inlineStr"/>
+      <c r="AX57" t="inlineStr"/>
+      <c r="AY57" t="inlineStr"/>
+      <c r="AZ57" t="inlineStr"/>
+      <c r="BA57" t="inlineStr"/>
+      <c r="BB57" t="inlineStr"/>
+      <c r="BC57" t="inlineStr"/>
+      <c r="BD57" t="inlineStr"/>
+      <c r="BE57" t="inlineStr"/>
+      <c r="BF57" t="inlineStr"/>
+      <c r="BG57" t="inlineStr"/>
+      <c r="BH57" t="inlineStr"/>
+      <c r="BI57" t="inlineStr"/>
+      <c r="BJ57" t="inlineStr"/>
+      <c r="BK57" t="inlineStr"/>
+      <c r="BL57" t="inlineStr"/>
+      <c r="BM57" t="inlineStr"/>
+      <c r="BN57" t="inlineStr"/>
+      <c r="BO57" t="inlineStr"/>
+      <c r="BP57" t="inlineStr"/>
+      <c r="BQ57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Antecipação de dividendos</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="n">
+        <v>30000</v>
+      </c>
+      <c r="F58" t="n">
+        <v>30000</v>
+      </c>
+      <c r="G58" t="n">
+        <v>30000</v>
+      </c>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
+      <c r="R58" t="inlineStr"/>
+      <c r="S58" t="inlineStr"/>
+      <c r="T58" t="inlineStr"/>
+      <c r="U58" t="inlineStr"/>
+      <c r="V58" t="inlineStr"/>
+      <c r="W58" t="inlineStr"/>
+      <c r="X58" t="inlineStr"/>
+      <c r="Y58" t="inlineStr"/>
+      <c r="Z58" t="inlineStr"/>
+      <c r="AA58" t="inlineStr"/>
+      <c r="AB58" t="inlineStr"/>
+      <c r="AC58" t="inlineStr"/>
+      <c r="AD58" t="inlineStr"/>
+      <c r="AE58" t="inlineStr"/>
+      <c r="AF58" t="inlineStr"/>
+      <c r="AG58" t="inlineStr"/>
+      <c r="AH58" t="inlineStr"/>
+      <c r="AI58" t="inlineStr"/>
+      <c r="AJ58" t="inlineStr"/>
+      <c r="AK58" t="inlineStr"/>
+      <c r="AL58" t="inlineStr"/>
+      <c r="AM58" t="inlineStr"/>
+      <c r="AN58" t="inlineStr"/>
+      <c r="AO58" t="inlineStr"/>
+      <c r="AP58" t="inlineStr"/>
+      <c r="AQ58" t="inlineStr"/>
+      <c r="AR58" t="inlineStr"/>
+      <c r="AS58" t="inlineStr"/>
+      <c r="AT58" t="inlineStr"/>
+      <c r="AU58" t="inlineStr"/>
+      <c r="AV58" t="inlineStr"/>
+      <c r="AW58" t="inlineStr"/>
+      <c r="AX58" t="inlineStr"/>
+      <c r="AY58" t="inlineStr"/>
+      <c r="AZ58" t="inlineStr"/>
+      <c r="BA58" t="inlineStr"/>
+      <c r="BB58" t="inlineStr"/>
+      <c r="BC58" t="inlineStr"/>
+      <c r="BD58" t="inlineStr"/>
+      <c r="BE58" t="inlineStr"/>
+      <c r="BF58" t="inlineStr"/>
+      <c r="BG58" t="inlineStr"/>
+      <c r="BH58" t="inlineStr"/>
+      <c r="BI58" t="inlineStr"/>
+      <c r="BJ58" t="inlineStr"/>
+      <c r="BK58" t="inlineStr"/>
+      <c r="BL58" t="inlineStr"/>
+      <c r="BM58" t="inlineStr"/>
+      <c r="BN58" t="inlineStr"/>
+      <c r="BO58" t="inlineStr"/>
+      <c r="BP58" t="inlineStr"/>
+      <c r="BQ58" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>